<commit_message>
DRS Data is current
</commit_message>
<xml_diff>
--- a/drs_data.xlsx
+++ b/drs_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harshvardhanuppaluru/Desktop/Personal/Cricket Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Desktop\Cricket-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D524A1-D7E6-BF40-A8F3-8D48854EF980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B37B87C-180B-4954-9FC4-3D8958DBAF3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21240" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2CB4CB80-56D3-FE4F-A149-B19EBDF0B673}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="145">
   <si>
     <t>Match</t>
   </si>
@@ -351,6 +349,126 @@
   </si>
   <si>
     <t>Bowler</t>
+  </si>
+  <si>
+    <t>Mustafizur Rahman</t>
+  </si>
+  <si>
+    <t>AS Joseph</t>
+  </si>
+  <si>
+    <t>TU Deshpande</t>
+  </si>
+  <si>
+    <t>C Green</t>
+  </si>
+  <si>
+    <t>HV Patel</t>
+  </si>
+  <si>
+    <t>Arshdeep Singh</t>
+  </si>
+  <si>
+    <t>AR Patel</t>
+  </si>
+  <si>
+    <t>M Markande</t>
+  </si>
+  <si>
+    <t>Harshit Rana</t>
+  </si>
+  <si>
+    <t>SP Narine</t>
+  </si>
+  <si>
+    <t>Ravi Bishnoi</t>
+  </si>
+  <si>
+    <t>Naveen-ul-Haq</t>
+  </si>
+  <si>
+    <t>Sandeep Sharma</t>
+  </si>
+  <si>
+    <t>Azmatullah Omarzai</t>
+  </si>
+  <si>
+    <t>R Sai Kishore</t>
+  </si>
+  <si>
+    <t>Mohammed Siraj</t>
+  </si>
+  <si>
+    <t>SM Curran</t>
+  </si>
+  <si>
+    <t>MM Sharma</t>
+  </si>
+  <si>
+    <t>DL Chahar</t>
+  </si>
+  <si>
+    <t>M Pathirana</t>
+  </si>
+  <si>
+    <t>G Coetzee</t>
+  </si>
+  <si>
+    <t>SZ Mulani</t>
+  </si>
+  <si>
+    <t>JD Unadkat</t>
+  </si>
+  <si>
+    <t>R Parag</t>
+  </si>
+  <si>
+    <t>Kuldeep Yadav</t>
+  </si>
+  <si>
+    <t>Mukesh Kumar</t>
+  </si>
+  <si>
+    <t>N Burger</t>
+  </si>
+  <si>
+    <t>Mohsin Khan</t>
+  </si>
+  <si>
+    <t>UT Yadav</t>
+  </si>
+  <si>
+    <t>Noor Ahmad</t>
+  </si>
+  <si>
+    <t>DG Nalkande</t>
+  </si>
+  <si>
+    <t>TA Boult</t>
+  </si>
+  <si>
+    <t>Q de Kock</t>
+  </si>
+  <si>
+    <t>Yash Dayal</t>
+  </si>
+  <si>
+    <t>RJW Topley</t>
+  </si>
+  <si>
+    <t>MP Yadav</t>
+  </si>
+  <si>
+    <t>Mohammad Siraj</t>
+  </si>
+  <si>
+    <t>PP Shaw</t>
+  </si>
+  <si>
+    <t>VG Arora</t>
+  </si>
+  <si>
+    <t>CV Varun</t>
   </si>
 </sst>
 </file>
@@ -396,10 +514,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -420,9 +538,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -460,7 +578,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -566,7 +684,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -708,7 +826,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -716,35 +834,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFF6E9B-8A82-B242-896A-8222911FE3F1}">
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="2"/>
-    <col min="4" max="4" width="7.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="2"/>
+    <col min="4" max="4" width="7.125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
     <col min="7" max="7" width="7" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="2"/>
-    <col min="9" max="9" width="23.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="2"/>
+    <col min="9" max="9" width="23.625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.375" style="2" customWidth="1"/>
     <col min="12" max="12" width="17.5" style="2" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="16" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="20.875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.25" style="2" customWidth="1"/>
     <col min="16" max="16" width="13" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="2"/>
+    <col min="17" max="17" width="13.875" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -797,7 +915,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -840,6 +958,9 @@
       <c r="N2" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="O2" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="P2" s="2" t="s">
         <v>103</v>
       </c>
@@ -847,7 +968,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -890,6 +1011,9 @@
       <c r="N3" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="O3" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="P3" s="2" t="s">
         <v>102</v>
       </c>
@@ -897,7 +1021,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -940,6 +1064,9 @@
       <c r="N4" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="O4" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="P4" s="2" t="s">
         <v>102</v>
       </c>
@@ -947,7 +1074,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -990,6 +1117,9 @@
       <c r="N5" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="O5" s="2" t="s">
+        <v>108</v>
+      </c>
       <c r="P5" s="2" t="s">
         <v>102</v>
       </c>
@@ -997,7 +1127,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1040,6 +1170,9 @@
       <c r="N6" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="O6" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="P6" s="2" t="s">
         <v>102</v>
       </c>
@@ -1047,7 +1180,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -1090,6 +1223,9 @@
       <c r="N7" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="O7" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="P7" s="2" t="s">
         <v>103</v>
       </c>
@@ -1097,7 +1233,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -1140,6 +1276,9 @@
       <c r="N8" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="O8" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="P8" s="2" t="s">
         <v>103</v>
       </c>
@@ -1147,7 +1286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -1190,6 +1329,9 @@
       <c r="N9" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="O9" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="P9" s="2" t="s">
         <v>102</v>
       </c>
@@ -1197,7 +1339,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -1240,6 +1382,9 @@
       <c r="N10" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="O10" s="2" t="s">
+        <v>111</v>
+      </c>
       <c r="P10" s="2" t="s">
         <v>102</v>
       </c>
@@ -1247,7 +1392,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -1290,6 +1435,9 @@
       <c r="N11" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="O11" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="P11" s="2" t="s">
         <v>103</v>
       </c>
@@ -1297,7 +1445,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -1340,6 +1488,9 @@
       <c r="N12" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="O12" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="P12" s="2" t="s">
         <v>103</v>
       </c>
@@ -1347,7 +1498,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -1390,6 +1541,9 @@
       <c r="N13" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="O13" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="P13" s="2" t="s">
         <v>102</v>
       </c>
@@ -1397,7 +1551,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>4</v>
       </c>
@@ -1440,6 +1594,9 @@
       <c r="N14" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="O14" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="P14" s="2" t="s">
         <v>103</v>
       </c>
@@ -1447,7 +1604,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -1490,6 +1647,9 @@
       <c r="N15" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="O15" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="P15" s="2" t="s">
         <v>102</v>
       </c>
@@ -1497,7 +1657,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>4</v>
       </c>
@@ -1540,6 +1700,9 @@
       <c r="N16" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="O16" s="2" t="s">
+        <v>116</v>
+      </c>
       <c r="P16" s="2" t="s">
         <v>102</v>
       </c>
@@ -1547,7 +1710,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>4</v>
       </c>
@@ -1590,6 +1753,9 @@
       <c r="N17" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="O17" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="P17" s="2" t="s">
         <v>102</v>
       </c>
@@ -1597,7 +1763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>5</v>
       </c>
@@ -1640,6 +1806,9 @@
       <c r="N18" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="O18" s="2" t="s">
+        <v>118</v>
+      </c>
       <c r="P18" s="2" t="s">
         <v>103</v>
       </c>
@@ -1647,7 +1816,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>5</v>
       </c>
@@ -1690,6 +1859,9 @@
       <c r="N19" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="O19" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="P19" s="2" t="s">
         <v>102</v>
       </c>
@@ -1697,7 +1869,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>6</v>
       </c>
@@ -1740,6 +1912,9 @@
       <c r="N20" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="O20" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="P20" s="2" t="s">
         <v>102</v>
       </c>
@@ -1747,7 +1922,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>6</v>
       </c>
@@ -1790,6 +1965,9 @@
       <c r="N21" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="O21" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="P21" s="2" t="s">
         <v>103</v>
       </c>
@@ -1797,7 +1975,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>6</v>
       </c>
@@ -1840,6 +2018,9 @@
       <c r="N22" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="O22" s="2" t="s">
+        <v>106</v>
+      </c>
       <c r="P22" s="2" t="s">
         <v>102</v>
       </c>
@@ -1847,7 +2028,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>6</v>
       </c>
@@ -1890,6 +2071,9 @@
       <c r="N23" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="O23" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="P23" s="2" t="s">
         <v>102</v>
       </c>
@@ -1897,7 +2081,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>6</v>
       </c>
@@ -1940,6 +2124,9 @@
       <c r="N24" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="O24" s="2" t="s">
+        <v>121</v>
+      </c>
       <c r="P24" s="2" t="s">
         <v>102</v>
       </c>
@@ -1947,7 +2134,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>7</v>
       </c>
@@ -1990,6 +2177,9 @@
       <c r="N25" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="O25" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="P25" s="2" t="s">
         <v>102</v>
       </c>
@@ -1997,7 +2187,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>7</v>
       </c>
@@ -2040,6 +2230,9 @@
       <c r="N26" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="O26" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="P26" s="2" t="s">
         <v>102</v>
       </c>
@@ -2047,7 +2240,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>7</v>
       </c>
@@ -2090,6 +2283,9 @@
       <c r="N27" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="O27" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="P27" s="2" t="s">
         <v>103</v>
       </c>
@@ -2097,7 +2293,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>7</v>
       </c>
@@ -2140,6 +2336,9 @@
       <c r="N28" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="O28" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="P28" s="2" t="s">
         <v>102</v>
       </c>
@@ -2147,7 +2346,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>7</v>
       </c>
@@ -2190,6 +2389,9 @@
       <c r="N29" s="2" t="s">
         <v>60</v>
       </c>
+      <c r="O29" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="P29" s="2" t="s">
         <v>103</v>
       </c>
@@ -2197,7 +2399,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>8</v>
       </c>
@@ -2240,6 +2442,9 @@
       <c r="N30" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="O30" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="P30" s="2" t="s">
         <v>102</v>
       </c>
@@ -2247,7 +2452,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>8</v>
       </c>
@@ -2290,6 +2495,9 @@
       <c r="N31" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="O31" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="P31" s="2" t="s">
         <v>102</v>
       </c>
@@ -2297,7 +2505,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>8</v>
       </c>
@@ -2340,6 +2548,9 @@
       <c r="N32" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="O32" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="P32" s="2" t="s">
         <v>102</v>
       </c>
@@ -2347,7 +2558,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>8</v>
       </c>
@@ -2390,6 +2601,9 @@
       <c r="N33" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="O33" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="P33" s="2" t="s">
         <v>102</v>
       </c>
@@ -2397,7 +2611,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>9</v>
       </c>
@@ -2440,6 +2654,9 @@
       <c r="N34" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="O34" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="P34" s="2" t="s">
         <v>103</v>
       </c>
@@ -2447,7 +2664,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>9</v>
       </c>
@@ -2488,7 +2705,10 @@
         <v>101</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>70</v>
+        <v>128</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="P35" s="2" t="s">
         <v>102</v>
@@ -2497,7 +2717,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>9</v>
       </c>
@@ -2540,6 +2760,9 @@
       <c r="N36" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="O36" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="P36" s="2" t="s">
         <v>102</v>
       </c>
@@ -2547,7 +2770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>9</v>
       </c>
@@ -2590,6 +2813,9 @@
       <c r="N37" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="O37" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="P37" s="2" t="s">
         <v>102</v>
       </c>
@@ -2597,7 +2823,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>10</v>
       </c>
@@ -2640,6 +2866,9 @@
       <c r="N38" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="O38" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="P38" s="2" t="s">
         <v>102</v>
       </c>
@@ -2647,7 +2876,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>11</v>
       </c>
@@ -2690,6 +2919,9 @@
       <c r="N39" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="O39" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="P39" s="2" t="s">
         <v>102</v>
       </c>
@@ -2697,7 +2929,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>12</v>
       </c>
@@ -2740,6 +2972,9 @@
       <c r="N40" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="O40" s="2" t="s">
+        <v>133</v>
+      </c>
       <c r="P40" s="2" t="s">
         <v>103</v>
       </c>
@@ -2747,7 +2982,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>12</v>
       </c>
@@ -2790,6 +3025,9 @@
       <c r="N41" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="O41" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="P41" s="2" t="s">
         <v>103</v>
       </c>
@@ -2797,7 +3035,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>12</v>
       </c>
@@ -2840,6 +3078,9 @@
       <c r="N42" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="O42" s="2" t="s">
+        <v>135</v>
+      </c>
       <c r="P42" s="2" t="s">
         <v>102</v>
       </c>
@@ -2847,7 +3088,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>13</v>
       </c>
@@ -2890,6 +3131,9 @@
       <c r="N43" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="O43" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="P43" s="2" t="s">
         <v>103</v>
       </c>
@@ -2897,7 +3141,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>14</v>
       </c>
@@ -2940,6 +3184,9 @@
       <c r="N44" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="O44" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="P44" s="2" t="s">
         <v>102</v>
       </c>
@@ -2947,7 +3194,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>14</v>
       </c>
@@ -2990,10 +3237,384 @@
       <c r="N45" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="O45" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="P45" s="2" t="s">
         <v>103</v>
       </c>
       <c r="Q45" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>15</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G46" s="2">
+        <v>15</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="P46" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q46" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>15</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" s="2">
+        <v>19</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="P47" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>15</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" s="2">
+        <v>20</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>15</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="2">
+        <v>2</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G49" s="2">
+        <v>15</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>15</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G50" s="2">
+        <v>19</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="P50" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q50" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>16</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="2">
+        <v>2</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G51" s="2">
+        <v>2</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O51" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="P51" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q51" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>16</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="2">
+        <v>2</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G52" s="2">
+        <v>13</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O52" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="P52" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q52" s="2" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>